<commit_message>
added well diameter sweep
</commit_message>
<xml_diff>
--- a/projects/virginia/parameter_sweep/user_inputs.xlsx
+++ b/projects/virginia/parameter_sweep/user_inputs.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864E33AA-BE25-4142-A539-86564FDAB831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041BB17E-DEA7-46F2-85B5-9EB12F849907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="low_k" sheetId="9" r:id="rId1"/>
     <sheet name="med_low_k" sheetId="16" r:id="rId2"/>
     <sheet name="med_high_k" sheetId="17" r:id="rId3"/>
     <sheet name="high_k" sheetId="15" r:id="rId4"/>
+    <sheet name="iowa_k" sheetId="18" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="22">
   <si>
     <t>Ref.</t>
   </si>
@@ -841,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CE3201-C3FB-49F0-971F-162DAF6B788A}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -1239,4 +1240,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F724D3C2-5C34-4460-84ED-CEBDE5C6F692}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1402.35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4">
+        <v>62.44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.22919999999999999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>